<commit_message>
some updates to tables for historic and future scenario simulations
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_EnergyCarrier_Price_CO2Emission.xlsx
+++ b/projects/test_building/input/Scenario_EnergyCarrier_Price_CO2Emission.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8592B4DB-2670-7548-A84E-8FE225358463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="-18220" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-180" yWindow="-18225" windowWidth="30240" windowHeight="17355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="note" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -181,7 +180,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -220,16 +219,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="33">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -341,55 +341,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:AT3" totalsRowShown="0">
-  <autoFilter ref="A1:AT3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AT3" totalsRowShown="0">
+  <autoFilter ref="A1:AT3"/>
   <tableColumns count="46">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_scenario"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="id_region"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="id_sector"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="unit"/>
-    <tableColumn id="38" xr3:uid="{31B57C8C-0C7C-154A-B0F0-1948F53F4D7A}" name="2010"/>
-    <tableColumn id="39" xr3:uid="{8BFD5C3B-2E3C-F74B-9EC7-DAB43053B3B6}" name="2011"/>
-    <tableColumn id="40" xr3:uid="{B906DD8F-3734-EC4F-821D-AAC415BF977C}" name="2012"/>
-    <tableColumn id="41" xr3:uid="{B5B5BBF7-F34E-604A-AB57-3B556C5B1D59}" name="2013"/>
-    <tableColumn id="42" xr3:uid="{19031027-ABA2-BD4C-8117-6AE0F17DFA8F}" name="2014"/>
-    <tableColumn id="43" xr3:uid="{B6703332-BF05-0E42-BDF4-748827D17BDE}" name="2015"/>
-    <tableColumn id="44" xr3:uid="{F4902D1A-A9ED-F14A-934B-25443D02A3DF}" name="2016"/>
-    <tableColumn id="45" xr3:uid="{92B1B26F-51E9-9144-AFFF-EEE8CA6E3BEC}" name="2017"/>
-    <tableColumn id="46" xr3:uid="{3783918F-3893-874A-9B13-D4D1F8E5E802}" name="2018"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="2019" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="2020" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="2021" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="2022" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="2023" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2024" dataDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="2025" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="2026" dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="2027" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="2028" dataDxfId="23"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="2029" dataDxfId="22"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="2030" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="2031" dataDxfId="20"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="2032" dataDxfId="19"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="2033" dataDxfId="18"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="2034" dataDxfId="17"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="2035" dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="2036" dataDxfId="15"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="2037" dataDxfId="14"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="2038" dataDxfId="13"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="2039" dataDxfId="12"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="2040" dataDxfId="11"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="2041" dataDxfId="10"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="2042" dataDxfId="9"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="2043" dataDxfId="8"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="2044" dataDxfId="7"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="2045" dataDxfId="6"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="2046" dataDxfId="5"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="2047" dataDxfId="4"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="2048" dataDxfId="3"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="2049" dataDxfId="2"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="2050" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{8D780864-D888-A648-921C-7F6063876797}" name="2051" dataDxfId="0"/>
+    <tableColumn id="1" name="id_scenario"/>
+    <tableColumn id="2" name="id_region"/>
+    <tableColumn id="3" name="id_sector"/>
+    <tableColumn id="5" name="unit"/>
+    <tableColumn id="38" name="2010"/>
+    <tableColumn id="39" name="2011"/>
+    <tableColumn id="40" name="2012"/>
+    <tableColumn id="41" name="2013"/>
+    <tableColumn id="42" name="2014"/>
+    <tableColumn id="43" name="2015"/>
+    <tableColumn id="44" name="2016"/>
+    <tableColumn id="45" name="2017"/>
+    <tableColumn id="46" name="2018"/>
+    <tableColumn id="6" name="2019" dataDxfId="32"/>
+    <tableColumn id="7" name="2020" dataDxfId="31"/>
+    <tableColumn id="8" name="2021" dataDxfId="30"/>
+    <tableColumn id="9" name="2022" dataDxfId="29"/>
+    <tableColumn id="10" name="2023" dataDxfId="28"/>
+    <tableColumn id="11" name="2024" dataDxfId="27"/>
+    <tableColumn id="12" name="2025" dataDxfId="26"/>
+    <tableColumn id="13" name="2026" dataDxfId="25"/>
+    <tableColumn id="14" name="2027" dataDxfId="24"/>
+    <tableColumn id="15" name="2028" dataDxfId="23"/>
+    <tableColumn id="16" name="2029" dataDxfId="22"/>
+    <tableColumn id="17" name="2030" dataDxfId="21"/>
+    <tableColumn id="18" name="2031" dataDxfId="20"/>
+    <tableColumn id="19" name="2032" dataDxfId="19"/>
+    <tableColumn id="20" name="2033" dataDxfId="18"/>
+    <tableColumn id="21" name="2034" dataDxfId="17"/>
+    <tableColumn id="22" name="2035" dataDxfId="16"/>
+    <tableColumn id="23" name="2036" dataDxfId="15"/>
+    <tableColumn id="24" name="2037" dataDxfId="14"/>
+    <tableColumn id="25" name="2038" dataDxfId="13"/>
+    <tableColumn id="26" name="2039" dataDxfId="12"/>
+    <tableColumn id="27" name="2040" dataDxfId="11"/>
+    <tableColumn id="28" name="2041" dataDxfId="10"/>
+    <tableColumn id="29" name="2042" dataDxfId="9"/>
+    <tableColumn id="30" name="2043" dataDxfId="8"/>
+    <tableColumn id="31" name="2044" dataDxfId="7"/>
+    <tableColumn id="32" name="2045" dataDxfId="6"/>
+    <tableColumn id="33" name="2046" dataDxfId="5"/>
+    <tableColumn id="34" name="2047" dataDxfId="4"/>
+    <tableColumn id="35" name="2048" dataDxfId="3"/>
+    <tableColumn id="36" name="2049" dataDxfId="2"/>
+    <tableColumn id="37" name="2050" dataDxfId="1"/>
+    <tableColumn id="4" name="2051" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -657,23 +657,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="AT6" sqref="AT6"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AT2" sqref="AT2:AT3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -813,7 +813,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -859,101 +859,101 @@
       <c r="O2" s="1">
         <v>0</v>
       </c>
-      <c r="P2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1">
-        <v>0</v>
-      </c>
-      <c r="T2" s="1">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1">
-        <v>0</v>
-      </c>
-      <c r="V2" s="1">
-        <v>0</v>
-      </c>
-      <c r="W2" s="1">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="1">
-        <v>0</v>
+      <c r="P2" s="2">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>30</v>
+      </c>
+      <c r="R2" s="2">
+        <v>35</v>
+      </c>
+      <c r="S2" s="2">
+        <v>45</v>
+      </c>
+      <c r="T2" s="2">
+        <v>55</v>
+      </c>
+      <c r="U2" s="2">
+        <v>57</v>
+      </c>
+      <c r="V2" s="2">
+        <v>60</v>
+      </c>
+      <c r="W2" s="2">
+        <v>62</v>
+      </c>
+      <c r="X2" s="2">
+        <v>64</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>65</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>84</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>83.808348127145933</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>86.158059642158435</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>88.433730600574123</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>90.641623163612849</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>92.787171856914142</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>94.875128470163503</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>96.909675952759088</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>98.894519037239718</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>100.83295714376011</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>102.72794361897078</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>104.58213431134067</v>
+      </c>
+      <c r="AP2" s="2">
+        <v>106.39792773605862</v>
+      </c>
+      <c r="AQ2" s="2">
+        <v>108.17749854124806</v>
+      </c>
+      <c r="AR2" s="2">
+        <v>109.92282559050837</v>
+      </c>
+      <c r="AS2" s="2">
+        <v>111.63571568246282</v>
+      </c>
+      <c r="AT2" s="2">
+        <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -999,98 +999,98 @@
       <c r="O3" s="1">
         <v>0</v>
       </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0</v>
-      </c>
-      <c r="V3" s="1">
-        <v>0</v>
-      </c>
-      <c r="W3" s="1">
-        <v>0</v>
-      </c>
-      <c r="X3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="1">
-        <v>0</v>
+      <c r="P3" s="2">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>30</v>
+      </c>
+      <c r="R3" s="2">
+        <v>35</v>
+      </c>
+      <c r="S3" s="2">
+        <v>45</v>
+      </c>
+      <c r="T3" s="2">
+        <v>55</v>
+      </c>
+      <c r="U3" s="2">
+        <v>57</v>
+      </c>
+      <c r="V3" s="2">
+        <v>60</v>
+      </c>
+      <c r="W3" s="2">
+        <v>62</v>
+      </c>
+      <c r="X3" s="2">
+        <v>64</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>65</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>67</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>84</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>83.808348127145933</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>86.158059642158435</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>88.433730600574123</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>90.641623163612849</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>92.787171856914142</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>94.875128470163503</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>96.909675952759088</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>98.894519037239718</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>100.83295714376011</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>102.72794361897078</v>
+      </c>
+      <c r="AO3" s="2">
+        <v>104.58213431134067</v>
+      </c>
+      <c r="AP3" s="2">
+        <v>106.39792773605862</v>
+      </c>
+      <c r="AQ3" s="2">
+        <v>108.17749854124806</v>
+      </c>
+      <c r="AR3" s="2">
+        <v>109.92282559050837</v>
+      </c>
+      <c r="AS3" s="2">
+        <v>111.63571568246282</v>
+      </c>
+      <c r="AT3" s="2">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1103,14 +1103,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BA2592-DA46-8345-B3AF-6776A9780F4B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>

</xml_diff>